<commit_message>
complete cell type hierarchy; map methods to the tree
</commit_message>
<xml_diff>
--- a/tables/cell_type_mapping2.xlsx
+++ b/tables/cell_type_mapping2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="44160" windowHeight="10275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="183">
   <si>
     <t xml:space="preserve">controlled vocabulary is a list of entities (cell types) of different granularity (e.g. T cell, CD8 T cell). We use this vocabulary to build a tree and to map cell type names between different methods/datasets. </t>
   </si>
@@ -167,13 +167,421 @@
   </si>
   <si>
     <t>cell</t>
+  </si>
+  <si>
+    <t>method_dataset</t>
+  </si>
+  <si>
+    <t>method_cell_type</t>
+  </si>
+  <si>
+    <t>cv_cell_type</t>
+  </si>
+  <si>
+    <t>B cells naive</t>
+  </si>
+  <si>
+    <t>B cells memory</t>
+  </si>
+  <si>
+    <t>Plasma cells</t>
+  </si>
+  <si>
+    <t>T cells CD8</t>
+  </si>
+  <si>
+    <t>T cells CD4 naive</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory resting</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory activated</t>
+  </si>
+  <si>
+    <t>NK cells resting</t>
+  </si>
+  <si>
+    <t>NK cells activated</t>
+  </si>
+  <si>
+    <t>Monocytes</t>
+  </si>
+  <si>
+    <t>Macrophages M0</t>
+  </si>
+  <si>
+    <t>Macrophages M1</t>
+  </si>
+  <si>
+    <t>Macrophages M2</t>
+  </si>
+  <si>
+    <t>Dendritic cells resting</t>
+  </si>
+  <si>
+    <t>Dendritic cells activated</t>
+  </si>
+  <si>
+    <t>Mast cells resting</t>
+  </si>
+  <si>
+    <t>Mast cells activated</t>
+  </si>
+  <si>
+    <t>Eosinophils</t>
+  </si>
+  <si>
+    <t>Neutrophils</t>
+  </si>
+  <si>
+    <t>CIBERSORT</t>
+  </si>
+  <si>
+    <t>B cell plasma</t>
+  </si>
+  <si>
+    <t>T cell follicular helper</t>
+  </si>
+  <si>
+    <t>T cell regulatory (Tregs)</t>
+  </si>
+  <si>
+    <t>T cell gamma delta</t>
+  </si>
+  <si>
+    <t>B_cell</t>
+  </si>
+  <si>
+    <t>T_cell.CD4</t>
+  </si>
+  <si>
+    <t>T_cell.CD8</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>TIMER</t>
+  </si>
+  <si>
+    <t>aDC</t>
+  </si>
+  <si>
+    <t>Adipocytes</t>
+  </si>
+  <si>
+    <t>Astrocytes</t>
+  </si>
+  <si>
+    <t>Basophils</t>
+  </si>
+  <si>
+    <t>B-cells</t>
+  </si>
+  <si>
+    <t>CD4+ memory T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ Tcm</t>
+  </si>
+  <si>
+    <t>CD4+ Tem</t>
+  </si>
+  <si>
+    <t>CD8+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ Tcm</t>
+  </si>
+  <si>
+    <t>CD8+ Tem</t>
+  </si>
+  <si>
+    <t>cDC</t>
+  </si>
+  <si>
+    <t>Chondrocytes</t>
+  </si>
+  <si>
+    <t>Class-switched memory B-cells</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>Endothelial cells</t>
+  </si>
+  <si>
+    <t>Epithelial cells</t>
+  </si>
+  <si>
+    <t>Erythrocytes</t>
+  </si>
+  <si>
+    <t>Fibroblasts</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Hepatocytes</t>
+  </si>
+  <si>
+    <t>HSC</t>
+  </si>
+  <si>
+    <t>iDC</t>
+  </si>
+  <si>
+    <t>Keratinocytes</t>
+  </si>
+  <si>
+    <t>ly Endothelial cells</t>
+  </si>
+  <si>
+    <t>Macrophages</t>
+  </si>
+  <si>
+    <t>Mast cells</t>
+  </si>
+  <si>
+    <t>Megakaryocytes</t>
+  </si>
+  <si>
+    <t>Melanocytes</t>
+  </si>
+  <si>
+    <t>Memory B-cells</t>
+  </si>
+  <si>
+    <t>MEP</t>
+  </si>
+  <si>
+    <t>Mesangial cells</t>
+  </si>
+  <si>
+    <t>MPP</t>
+  </si>
+  <si>
+    <t>MSC</t>
+  </si>
+  <si>
+    <t>mv Endothelial cells</t>
+  </si>
+  <si>
+    <t>Myocytes</t>
+  </si>
+  <si>
+    <t>naive B-cells</t>
+  </si>
+  <si>
+    <t>Neurons</t>
+  </si>
+  <si>
+    <t>NK cells</t>
+  </si>
+  <si>
+    <t>NKT</t>
+  </si>
+  <si>
+    <t>Osteoblast</t>
+  </si>
+  <si>
+    <t>pDC</t>
+  </si>
+  <si>
+    <t>Pericytes</t>
+  </si>
+  <si>
+    <t>Platelets</t>
+  </si>
+  <si>
+    <t>Preadipocytes</t>
+  </si>
+  <si>
+    <t>pro B-cells</t>
+  </si>
+  <si>
+    <t>Sebocytes</t>
+  </si>
+  <si>
+    <t>Skeletal muscle</t>
+  </si>
+  <si>
+    <t>Smooth muscle</t>
+  </si>
+  <si>
+    <t>Tgd cells</t>
+  </si>
+  <si>
+    <t>Th1 cells</t>
+  </si>
+  <si>
+    <t>Th2 cells</t>
+  </si>
+  <si>
+    <t>Tregs</t>
+  </si>
+  <si>
+    <t>ImmuneScore</t>
+  </si>
+  <si>
+    <t>StromaScore</t>
+  </si>
+  <si>
+    <t>MicroenvironmentScore</t>
+  </si>
+  <si>
+    <t>xCell</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>MCP counter</t>
+  </si>
+  <si>
+    <t>T cells</t>
+  </si>
+  <si>
+    <t>CD8 T cells</t>
+  </si>
+  <si>
+    <t>Cytotoxic lymphocytes</t>
+  </si>
+  <si>
+    <t>B lineage</t>
+  </si>
+  <si>
+    <t>Myeloid dendritic cells</t>
+  </si>
+  <si>
+    <t>B.cells</t>
+  </si>
+  <si>
+    <t>Macrophages.M1</t>
+  </si>
+  <si>
+    <t>Macrophages.M2</t>
+  </si>
+  <si>
+    <t>NK.cells</t>
+  </si>
+  <si>
+    <t>T.cells.CD4</t>
+  </si>
+  <si>
+    <t>T.cells.CD8</t>
+  </si>
+  <si>
+    <t>Dendritic.cells</t>
+  </si>
+  <si>
+    <t>quanTIseq</t>
+  </si>
+  <si>
+    <t>Bcells</t>
+  </si>
+  <si>
+    <t>CAFs</t>
+  </si>
+  <si>
+    <t>CD4_Tcells</t>
+  </si>
+  <si>
+    <t>CD8_Tcells</t>
+  </si>
+  <si>
+    <t>Endothelial</t>
+  </si>
+  <si>
+    <t>NKcells</t>
+  </si>
+  <si>
+    <t>otherCells</t>
+  </si>
+  <si>
+    <t>EPIC</t>
+  </si>
+  <si>
+    <t>B cells</t>
+  </si>
+  <si>
+    <t>CD8+ T cells</t>
+  </si>
+  <si>
+    <t>Melanoma cells</t>
+  </si>
+  <si>
+    <t>CD4+ T cells</t>
+  </si>
+  <si>
+    <t>Macrophages/Monocytes</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>regulatory T cells</t>
+  </si>
+  <si>
+    <t>Cancer associated fibroblasts</t>
+  </si>
+  <si>
+    <t>Dendritic cells</t>
+  </si>
+  <si>
+    <t>Natural killer cells</t>
+  </si>
+  <si>
+    <t>Ovarian carcinoma cells</t>
+  </si>
+  <si>
+    <t>schelker_single_cell</t>
+  </si>
+  <si>
+    <t>Macrophage/Monocyte</t>
+  </si>
+  <si>
+    <t>Tcell</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>mono</t>
+  </si>
+  <si>
+    <t>hoeck</t>
+  </si>
+  <si>
+    <t>CD4 T cells</t>
+  </si>
+  <si>
+    <t>cancer cells</t>
+  </si>
+  <si>
+    <t>racle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +604,20 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,10 +639,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,16 +988,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
     <col min="4" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
@@ -645,7 +1098,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -654,7 +1107,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -663,7 +1116,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -702,25 +1155,25 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>12</v>
@@ -729,25 +1182,25 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -756,7 +1209,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -765,16 +1218,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -783,25 +1236,25 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>175</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>29</v>
@@ -810,23 +1263,24 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
@@ -834,55 +1288,55 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -890,23 +1344,39 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3:B35 B37:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B1048576 B30:B37 B3:B28 B1">
       <formula1>$A:$A</formula1>
     </dataValidation>
   </dataValidations>
@@ -917,13 +1387,1485 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C102" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C105" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C106" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C111" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C112" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C113" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C115" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C116" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>162</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C117" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C118" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C121" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C122" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C123" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>174</v>
+      </c>
+      <c r="B125" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C125" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B127" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C127" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B129" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C129" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B130" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B131" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C131" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C132" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C133" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C134" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B135" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B136" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C136" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>179</v>
+      </c>
+      <c r="B137" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B138" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C138" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B139" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B140" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C140" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B141" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>182</v>
+      </c>
+      <c r="B142" t="s">
+        <v>163</v>
+      </c>
+      <c r="C142" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B143" t="s">
+        <v>180</v>
+      </c>
+      <c r="C143" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B144" t="s">
+        <v>143</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B145" t="s">
+        <v>121</v>
+      </c>
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B146" t="s">
+        <v>181</v>
+      </c>
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>controlled_vocabulary!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>